<commit_message>
using CaseUtil and RestUtil
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase_v3.xlsx
+++ b/src/test/resources/TestCase_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaa./Documents/project/apiAuto/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F848A7-AF05-6341-89BC-409516AF412C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAECF11-3C69-924D-BAA8-13BD4E06ED99}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="460" windowWidth="27840" windowHeight="17040" activeTab="1" xr2:uid="{C4640F5E-EB96-FA47-A8DC-E82707FAD38B}"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="27840" windowHeight="17040" xr2:uid="{C4640F5E-EB96-FA47-A8DC-E82707FAD38B}"/>
   </bookViews>
   <sheets>
     <sheet name="ApiInfoSheet" sheetId="1" r:id="rId1"/>
@@ -31,19 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
-  <si>
-    <t>ApiId</t>
-  </si>
-  <si>
-    <t>APIName</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Url</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>register</t>
   </si>
@@ -193,6 +181,15 @@
   </si>
   <si>
     <t>Desc(用例描述)</t>
+  </si>
+  <si>
+    <t>Type(接口提交方式)</t>
+  </si>
+  <si>
+    <t>Url(接口地址)</t>
+  </si>
+  <si>
+    <t>ApiName(接口名称)</t>
   </si>
 </sst>
 </file>
@@ -549,30 +546,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9095769F-B6B7-B544-AFF2-ECAA0DF6AF7B}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="69.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -580,13 +577,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -594,13 +591,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -608,13 +605,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -622,13 +619,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -636,13 +633,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -650,13 +647,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -664,13 +661,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -678,13 +675,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -692,13 +689,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -706,13 +703,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -720,13 +717,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -734,13 +731,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -748,13 +745,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -766,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566387FB-5D5B-5647-B138-BF28E6EAB354}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -780,16 +777,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -800,10 +797,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -814,10 +811,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -828,10 +825,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -842,10 +839,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -856,10 +853,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -870,10 +867,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -884,10 +881,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -898,10 +895,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -912,10 +909,10 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -926,10 +923,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -940,10 +937,10 @@
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>